<commit_message>
Now you can add new prices, and you can also get the price list. response.py is also changed so you get the username
</commit_message>
<xml_diff>
--- a/prices.xlsx
+++ b/prices.xlsx
@@ -1,42 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d9507a098afb7cda/math/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thien\Desktop\coding_projects\Mathbot_real\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{75815B0D-88F1-495D-943F-3EC95786AA0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82D58141-8CA5-438D-BEB5-50831B61864F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CA48C0-2BFD-47AC-A894-10900273C65E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="444" yWindow="0" windowWidth="17232" windowHeight="12012" xr2:uid="{009365B7-2CEF-4061-B90C-90F9134AB4E0}"/>
+    <workbookView xWindow="0" yWindow="228" windowWidth="17220" windowHeight="12012" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+  <si>
+    <t>Hat</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
   <si>
     <t>Abraham Lincoln</t>
   </si>
@@ -116,23 +106,25 @@
     <t>Vaskespray</t>
   </si>
   <si>
-    <t>Hat</t>
-  </si>
-  <si>
-    <t>Price</t>
+    <t>Gjøgler pacman lilla</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -155,8 +147,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -172,6 +165,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B28" totalsRowShown="0">
+  <autoFilter ref="A1:B28" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B28">
+    <sortCondition ref="A1:A28"/>
+  </sortState>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Hat"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Price"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -470,11 +477,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B696DA87-FF0E-477F-AD81-F22EC57A760E}">
-  <dimension ref="A1:B27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -484,15 +491,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>2500</v>
@@ -500,7 +507,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>100</v>
@@ -508,7 +515,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>500</v>
@@ -516,7 +523,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>550</v>
@@ -524,7 +531,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>500</v>
@@ -532,7 +539,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>750</v>
@@ -540,7 +547,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>100</v>
@@ -548,7 +555,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>650</v>
@@ -556,63 +563,63 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>700</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>9</v>
+      <c r="A11" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="B11">
-        <v>800</v>
+        <v>5200</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>600</v>
+        <v>800</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>300</v>
+        <v>600</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14">
-        <v>3500</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <v>150</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>300</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>300</v>
@@ -620,86 +627,97 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18">
-        <v>1200</v>
+        <v>300</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>250</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20">
-        <v>550</v>
+        <v>250</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21">
-        <v>200</v>
+        <v>550</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22">
-        <v>500</v>
+        <v>200</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23">
-        <v>150</v>
+        <v>500</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24">
-        <v>75</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25">
-        <v>1500</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26">
-        <v>875</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed and cleaned it for math questions
</commit_message>
<xml_diff>
--- a/prices.xlsx
+++ b/prices.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thien\Desktop\coding_projects\Mathbot_real\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CA48C0-2BFD-47AC-A894-10900273C65E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9187F6E0-14D0-4BC8-8587-49C2DCAA66A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="228" windowWidth="17220" windowHeight="12012" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4188" yWindow="228" windowWidth="18852" windowHeight="12012" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -55,6 +55,9 @@
     <t>Giftering med diamant</t>
   </si>
   <si>
+    <t>Gjøgler pacman lilla</t>
+  </si>
+  <si>
     <t>Gjøglertiss</t>
   </si>
   <si>
@@ -104,9 +107,6 @@
   </si>
   <si>
     <t>Vaskespray</t>
-  </si>
-  <si>
-    <t>Gjøgler pacman lilla</t>
   </si>
 </sst>
 </file>
@@ -480,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B33" sqref="A29:B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -571,7 +571,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>5200</v>
@@ -579,7 +579,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>800</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13">
         <v>600</v>
@@ -595,7 +595,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14">
         <v>300</v>
@@ -603,7 +603,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15">
         <v>3500</v>
@@ -611,7 +611,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16">
         <v>150</v>
@@ -619,7 +619,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17">
         <v>300</v>
@@ -627,7 +627,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18">
         <v>300</v>
@@ -635,7 +635,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19">
         <v>1200</v>
@@ -643,7 +643,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20">
         <v>250</v>
@@ -651,7 +651,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21">
         <v>550</v>
@@ -659,7 +659,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22">
         <v>200</v>
@@ -667,7 +667,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23">
         <v>500</v>
@@ -675,7 +675,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24">
         <v>150</v>
@@ -683,7 +683,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25">
         <v>75</v>
@@ -691,7 +691,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26">
         <v>1500</v>
@@ -699,7 +699,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27">
         <v>875</v>
@@ -707,7 +707,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28">
         <v>25</v>

</xml_diff>